<commit_message>
stuff to be committed
</commit_message>
<xml_diff>
--- a/Lab0_Alex/odometryMeasurements.xlsx
+++ b/Lab0_Alex/odometryMeasurements.xlsx
@@ -359,7 +359,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +394,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
       <c r="C3">
         <v>4.5</v>

</xml_diff>